<commit_message>
home and test versions work
</commit_message>
<xml_diff>
--- a/calendar_school.xlsx
+++ b/calendar_school.xlsx
@@ -35,8 +35,8 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00DBBCD3"/>
-        <bgColor rgb="00DBBCD3"/>
+        <fgColor rgb="00633535"/>
+        <bgColor rgb="00633535"/>
       </patternFill>
     </fill>
     <fill>
@@ -47,14 +47,14 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00BCDBC4"/>
-        <bgColor rgb="00BCDBC4"/>
+        <fgColor rgb="00DBBCD3"/>
+        <bgColor rgb="00DBBCD3"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00356363"/>
-        <bgColor rgb="00356363"/>
+        <fgColor rgb="00F4E0A3"/>
+        <bgColor rgb="00F4E0A3"/>
       </patternFill>
     </fill>
     <fill>
@@ -65,20 +65,20 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00F4E0A3"/>
-        <bgColor rgb="00F4E0A3"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00633535"/>
-        <bgColor rgb="00633535"/>
+        <fgColor rgb="00BCDBC4"/>
+        <bgColor rgb="00BCDBC4"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="004C0F89"/>
         <bgColor rgb="004C0F89"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00356363"/>
+        <bgColor rgb="00356363"/>
       </patternFill>
     </fill>
   </fills>
@@ -100,10 +100,10 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -551,448 +551,401 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="n"/>
-      <c r="B1" s="2" t="n"/>
+      <c r="B1" s="1" t="n"/>
       <c r="C1" s="2" t="n"/>
-      <c r="E1" s="2" t="n"/>
+      <c r="E1" s="3" t="n"/>
       <c r="F1" s="3" t="n"/>
       <c r="G1" s="3" t="n"/>
-      <c r="H1" s="3" t="n"/>
-      <c r="I1" s="3" t="n"/>
-      <c r="J1" s="3" t="n"/>
-      <c r="M1" s="4" t="n"/>
-      <c r="N1" s="4" t="n"/>
+      <c r="H1" s="4" t="n"/>
+      <c r="J1" s="4" t="n"/>
+      <c r="M1" s="3" t="n"/>
+      <c r="N1" s="3" t="n"/>
       <c r="O1" s="3" t="n"/>
       <c r="Q1" s="5" t="n"/>
       <c r="R1" s="5" t="n"/>
-      <c r="S1" s="5" t="n"/>
-      <c r="T1" s="5" t="n"/>
-      <c r="U1" s="5" t="n"/>
-      <c r="V1" s="1" t="n"/>
-      <c r="Y1" s="3" t="n"/>
-      <c r="Z1" s="3" t="n"/>
-      <c r="AA1" s="5" t="n"/>
-      <c r="AC1" s="4" t="n"/>
-      <c r="AD1" s="4" t="n"/>
-      <c r="AE1" s="4" t="n"/>
+      <c r="S1" s="1" t="n"/>
+      <c r="T1" s="1" t="n"/>
+      <c r="V1" s="6" t="n"/>
+      <c r="Y1" s="1" t="n"/>
+      <c r="Z1" s="1" t="n"/>
+      <c r="AA1" s="1" t="n"/>
+      <c r="AC1" s="3" t="n"/>
+      <c r="AD1" s="3" t="n"/>
+      <c r="AE1" s="3" t="n"/>
       <c r="AF1" s="4" t="n"/>
-      <c r="AG1" s="6" t="n"/>
-      <c r="AH1" s="6" t="n"/>
-      <c r="AK1" s="1" t="n"/>
-      <c r="AL1" s="1" t="n"/>
-      <c r="AM1" s="1" t="n"/>
-      <c r="AO1" s="7" t="n"/>
-      <c r="AP1" s="5" t="n"/>
-      <c r="AQ1" s="5" t="n"/>
-      <c r="AR1" s="5" t="n"/>
-      <c r="AS1" s="5" t="n"/>
-      <c r="AT1" s="5" t="n"/>
+      <c r="AH1" s="4" t="n"/>
+      <c r="AK1" s="3" t="n"/>
+      <c r="AL1" s="3" t="n"/>
+      <c r="AM1" s="3" t="n"/>
+      <c r="AO1" s="5" t="n"/>
+      <c r="AP1" s="4" t="n"/>
+      <c r="AQ1" s="7" t="n"/>
+      <c r="AR1" s="7" t="n"/>
+      <c r="AT1" s="6" t="n"/>
       <c r="AW1" s="3" t="n"/>
       <c r="AX1" s="3" t="n"/>
-      <c r="AY1" s="8" t="n"/>
+      <c r="AY1" s="3" t="n"/>
       <c r="BA1" s="8" t="n"/>
-      <c r="BB1" s="4" t="n"/>
-      <c r="BC1" s="2" t="n"/>
-      <c r="BD1" s="6" t="n"/>
-      <c r="BE1" s="6" t="n"/>
+      <c r="BB1" s="8" t="n"/>
+      <c r="BC1" s="1" t="n"/>
+      <c r="BD1" s="1" t="n"/>
       <c r="BF1" s="6" t="n"/>
-      <c r="BI1" s="1" t="n"/>
-      <c r="BJ1" s="1" t="n"/>
-      <c r="BK1" s="1" t="n"/>
-      <c r="BM1" s="7" t="n"/>
-      <c r="BN1" s="5" t="n"/>
-      <c r="BO1" s="5" t="n"/>
-      <c r="BP1" s="5" t="n"/>
-      <c r="BQ1" s="5" t="n"/>
-      <c r="BR1" s="5" t="n"/>
+      <c r="BI1" s="3" t="n"/>
+      <c r="BJ1" s="3" t="n"/>
+      <c r="BK1" s="3" t="n"/>
+      <c r="BM1" s="6" t="n"/>
+      <c r="BN1" s="4" t="n"/>
+      <c r="BO1" s="4" t="n"/>
+      <c r="BP1" s="7" t="n"/>
+      <c r="BR1" s="7" t="n"/>
     </row>
     <row r="2">
       <c r="A2" s="1" t="n"/>
       <c r="B2" s="1" t="n"/>
       <c r="C2" s="2" t="n"/>
       <c r="D2" s="2" t="n"/>
-      <c r="E2" s="2" t="n"/>
+      <c r="E2" s="3" t="n"/>
       <c r="F2" s="3" t="n"/>
       <c r="G2" s="4" t="n"/>
       <c r="H2" s="4" t="n"/>
       <c r="I2" s="4" t="n"/>
       <c r="J2" s="4" t="n"/>
-      <c r="M2" s="4" t="n"/>
-      <c r="N2" s="4" t="n"/>
-      <c r="O2" s="3" t="n"/>
-      <c r="P2" s="3" t="n"/>
-      <c r="Q2" s="3" t="n"/>
-      <c r="R2" s="3" t="n"/>
-      <c r="S2" s="3" t="n"/>
-      <c r="T2" s="5" t="n"/>
-      <c r="U2" s="1" t="n"/>
-      <c r="V2" s="1" t="n"/>
-      <c r="Y2" s="3" t="n"/>
-      <c r="Z2" s="5" t="n"/>
-      <c r="AA2" s="5" t="n"/>
-      <c r="AB2" s="5" t="n"/>
-      <c r="AC2" s="5" t="n"/>
-      <c r="AD2" s="5" t="n"/>
+      <c r="M2" s="3" t="n"/>
+      <c r="N2" s="3" t="n"/>
+      <c r="O2" s="4" t="n"/>
+      <c r="P2" s="4" t="n"/>
+      <c r="Q2" s="5" t="n"/>
+      <c r="R2" s="8" t="n"/>
+      <c r="S2" s="1" t="n"/>
+      <c r="T2" s="1" t="n"/>
+      <c r="U2" s="2" t="n"/>
+      <c r="V2" s="6" t="n"/>
+      <c r="Y2" s="1" t="n"/>
+      <c r="Z2" s="1" t="n"/>
+      <c r="AA2" s="2" t="n"/>
+      <c r="AB2" s="2" t="n"/>
+      <c r="AC2" s="3" t="n"/>
+      <c r="AD2" s="3" t="n"/>
       <c r="AE2" s="4" t="n"/>
       <c r="AF2" s="4" t="n"/>
-      <c r="AG2" s="6" t="n"/>
-      <c r="AH2" s="6" t="n"/>
-      <c r="AK2" s="1" t="n"/>
-      <c r="AL2" s="1" t="n"/>
-      <c r="AM2" s="7" t="n"/>
-      <c r="AN2" s="7" t="n"/>
-      <c r="AO2" s="7" t="n"/>
+      <c r="AG2" s="4" t="n"/>
+      <c r="AH2" s="4" t="n"/>
+      <c r="AK2" s="2" t="n"/>
+      <c r="AL2" s="3" t="n"/>
+      <c r="AM2" s="3" t="n"/>
+      <c r="AN2" s="8" t="n"/>
+      <c r="AO2" s="5" t="n"/>
       <c r="AP2" s="4" t="n"/>
-      <c r="AQ2" s="2" t="n"/>
-      <c r="AR2" s="2" t="n"/>
-      <c r="AS2" s="5" t="n"/>
-      <c r="AT2" s="2" t="n"/>
+      <c r="AQ2" s="4" t="n"/>
+      <c r="AR2" s="7" t="n"/>
+      <c r="AS2" s="6" t="n"/>
+      <c r="AT2" s="6" t="n"/>
       <c r="AW2" s="3" t="n"/>
-      <c r="AX2" s="8" t="n"/>
-      <c r="AY2" s="8" t="n"/>
-      <c r="AZ2" s="8" t="n"/>
+      <c r="AX2" s="3" t="n"/>
+      <c r="AY2" s="4" t="n"/>
+      <c r="AZ2" s="4" t="n"/>
       <c r="BA2" s="8" t="n"/>
-      <c r="BB2" s="4" t="n"/>
-      <c r="BC2" s="2" t="n"/>
-      <c r="BD2" s="2" t="n"/>
+      <c r="BB2" s="8" t="n"/>
+      <c r="BC2" s="1" t="n"/>
+      <c r="BD2" s="1" t="n"/>
       <c r="BE2" s="6" t="n"/>
       <c r="BF2" s="6" t="n"/>
-      <c r="BI2" s="1" t="n"/>
-      <c r="BJ2" s="1" t="n"/>
-      <c r="BK2" s="7" t="n"/>
-      <c r="BL2" s="7" t="n"/>
-      <c r="BM2" s="7" t="n"/>
-      <c r="BN2" s="4" t="n"/>
-      <c r="BO2" s="2" t="n"/>
-      <c r="BP2" s="2" t="n"/>
-      <c r="BQ2" s="5" t="n"/>
-      <c r="BR2" s="2" t="n"/>
+      <c r="BI2" s="2" t="n"/>
+      <c r="BJ2" s="3" t="n"/>
+      <c r="BK2" s="3" t="n"/>
+      <c r="BL2" s="8" t="n"/>
+      <c r="BM2" s="6" t="n"/>
+      <c r="BN2" s="6" t="n"/>
+      <c r="BO2" s="4" t="n"/>
+      <c r="BP2" s="7" t="n"/>
+      <c r="BQ2" s="7" t="n"/>
+      <c r="BR2" s="7" t="n"/>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n"/>
-      <c r="B3" s="1" t="n"/>
-      <c r="C3" s="1" t="n"/>
-      <c r="D3" s="7" t="n"/>
-      <c r="E3" s="7" t="n"/>
-      <c r="F3" s="8" t="n"/>
-      <c r="H3" s="8" t="n"/>
-      <c r="I3" s="4" t="n"/>
-      <c r="J3" s="4" t="n"/>
-      <c r="M3" s="4" t="n"/>
+      <c r="B3" s="7" t="n"/>
+      <c r="C3" s="7" t="n"/>
+      <c r="D3" s="2" t="n"/>
+      <c r="E3" s="3" t="n"/>
+      <c r="F3" s="5" t="n"/>
+      <c r="G3" s="5" t="n"/>
+      <c r="H3" s="5" t="n"/>
+      <c r="I3" s="5" t="n"/>
+      <c r="J3" s="5" t="n"/>
+      <c r="M3" s="3" t="n"/>
       <c r="N3" s="7" t="n"/>
       <c r="O3" s="7" t="n"/>
-      <c r="P3" s="2" t="n"/>
-      <c r="Q3" s="2" t="n"/>
-      <c r="R3" s="2" t="n"/>
-      <c r="T3" s="1" t="n"/>
-      <c r="U3" s="1" t="n"/>
-      <c r="V3" s="1" t="n"/>
-      <c r="Y3" s="3" t="n"/>
-      <c r="Z3" s="1" t="n"/>
-      <c r="AA3" s="8" t="n"/>
-      <c r="AB3" s="8" t="n"/>
-      <c r="AC3" s="8" t="n"/>
-      <c r="AD3" s="8" t="n"/>
-      <c r="AF3" s="7" t="n"/>
-      <c r="AG3" s="7" t="n"/>
-      <c r="AH3" s="6" t="n"/>
-      <c r="AK3" s="1" t="n"/>
-      <c r="AL3" s="8" t="n"/>
-      <c r="AM3" s="7" t="n"/>
+      <c r="P3" s="4" t="n"/>
+      <c r="Q3" s="5" t="n"/>
+      <c r="R3" s="8" t="n"/>
+      <c r="S3" s="1" t="n"/>
+      <c r="T3" s="2" t="n"/>
+      <c r="U3" s="2" t="n"/>
+      <c r="V3" s="6" t="n"/>
+      <c r="Y3" s="7" t="n"/>
+      <c r="Z3" s="7" t="n"/>
+      <c r="AA3" s="7" t="n"/>
+      <c r="AB3" s="2" t="n"/>
+      <c r="AC3" s="3" t="n"/>
+      <c r="AD3" s="5" t="n"/>
+      <c r="AE3" s="5" t="n"/>
+      <c r="AF3" s="5" t="n"/>
+      <c r="AG3" s="5" t="n"/>
+      <c r="AH3" s="5" t="n"/>
+      <c r="AK3" s="2" t="n"/>
+      <c r="AL3" s="2" t="n"/>
+      <c r="AM3" s="3" t="n"/>
       <c r="AN3" s="8" t="n"/>
-      <c r="AO3" s="7" t="n"/>
+      <c r="AO3" s="5" t="n"/>
       <c r="AP3" s="4" t="n"/>
-      <c r="AR3" s="2" t="n"/>
-      <c r="AS3" s="2" t="n"/>
-      <c r="AT3" s="2" t="n"/>
+      <c r="AQ3" s="7" t="n"/>
+      <c r="AR3" s="7" t="n"/>
+      <c r="AS3" s="7" t="n"/>
+      <c r="AT3" s="6" t="n"/>
       <c r="AW3" s="3" t="n"/>
-      <c r="AX3" s="1" t="n"/>
-      <c r="AY3" s="1" t="n"/>
-      <c r="AZ3" s="1" t="n"/>
-      <c r="BA3" s="4" t="n"/>
-      <c r="BB3" s="4" t="n"/>
+      <c r="AX3" s="7" t="n"/>
+      <c r="AY3" s="7" t="n"/>
+      <c r="AZ3" s="4" t="n"/>
+      <c r="BA3" s="8" t="n"/>
+      <c r="BB3" s="2" t="n"/>
+      <c r="BC3" s="1" t="n"/>
       <c r="BD3" s="2" t="n"/>
-      <c r="BE3" s="7" t="n"/>
-      <c r="BF3" s="7" t="n"/>
-      <c r="BI3" s="1" t="n"/>
-      <c r="BJ3" s="8" t="n"/>
-      <c r="BK3" s="7" t="n"/>
+      <c r="BE3" s="2" t="n"/>
+      <c r="BF3" s="6" t="n"/>
+      <c r="BI3" s="2" t="n"/>
+      <c r="BJ3" s="2" t="n"/>
+      <c r="BK3" s="3" t="n"/>
       <c r="BL3" s="8" t="n"/>
-      <c r="BM3" s="7" t="n"/>
+      <c r="BM3" s="6" t="n"/>
       <c r="BN3" s="4" t="n"/>
-      <c r="BP3" s="2" t="n"/>
-      <c r="BQ3" s="2" t="n"/>
-      <c r="BR3" s="2" t="n"/>
+      <c r="BO3" s="4" t="n"/>
+      <c r="BP3" s="1" t="n"/>
+      <c r="BQ3" s="1" t="n"/>
+      <c r="BR3" s="7" t="n"/>
     </row>
     <row r="4">
-      <c r="A4" s="6" t="n"/>
-      <c r="B4" s="6" t="n"/>
-      <c r="C4" s="6" t="n"/>
-      <c r="D4" s="7" t="n"/>
-      <c r="E4" s="8" t="n"/>
-      <c r="F4" s="8" t="n"/>
+      <c r="B4" s="7" t="n"/>
+      <c r="C4" s="2" t="n"/>
+      <c r="D4" s="2" t="n"/>
+      <c r="E4" s="6" t="n"/>
+      <c r="F4" s="5" t="n"/>
       <c r="G4" s="8" t="n"/>
       <c r="H4" s="8" t="n"/>
-      <c r="I4" s="5" t="n"/>
-      <c r="M4" s="4" t="n"/>
+      <c r="I4" s="8" t="n"/>
+      <c r="J4" s="8" t="n"/>
       <c r="N4" s="7" t="n"/>
-      <c r="O4" s="2" t="n"/>
-      <c r="P4" s="2" t="n"/>
-      <c r="Q4" s="8" t="n"/>
-      <c r="R4" s="2" t="n"/>
+      <c r="O4" s="4" t="n"/>
+      <c r="P4" s="4" t="n"/>
+      <c r="Q4" s="5" t="n"/>
+      <c r="R4" s="8" t="n"/>
       <c r="S4" s="8" t="n"/>
-      <c r="T4" s="6" t="n"/>
+      <c r="T4" s="2" t="n"/>
       <c r="U4" s="6" t="n"/>
-      <c r="Y4" s="3" t="n"/>
-      <c r="Z4" s="1" t="n"/>
-      <c r="AA4" s="1" t="n"/>
-      <c r="AB4" s="8" t="n"/>
-      <c r="AC4" s="2" t="n"/>
-      <c r="AD4" s="8" t="n"/>
-      <c r="AE4" s="2" t="n"/>
-      <c r="AF4" s="2" t="n"/>
-      <c r="AG4" s="7" t="n"/>
-      <c r="AK4" s="3" t="n"/>
-      <c r="AL4" s="8" t="n"/>
+      <c r="V4" s="6" t="n"/>
+      <c r="Z4" s="7" t="n"/>
+      <c r="AA4" s="2" t="n"/>
+      <c r="AB4" s="2" t="n"/>
+      <c r="AC4" s="6" t="n"/>
+      <c r="AD4" s="5" t="n"/>
+      <c r="AE4" s="8" t="n"/>
+      <c r="AF4" s="8" t="n"/>
+      <c r="AG4" s="8" t="n"/>
+      <c r="AH4" s="8" t="n"/>
+      <c r="AL4" s="2" t="n"/>
       <c r="AM4" s="8" t="n"/>
       <c r="AN4" s="8" t="n"/>
-      <c r="AO4" s="8" t="n"/>
+      <c r="AO4" s="5" t="n"/>
       <c r="AP4" s="4" t="n"/>
       <c r="AQ4" s="4" t="n"/>
-      <c r="AR4" s="6" t="n"/>
-      <c r="AS4" s="6" t="n"/>
-      <c r="AW4" s="3" t="n"/>
-      <c r="AX4" s="1" t="n"/>
-      <c r="AY4" s="1" t="n"/>
-      <c r="AZ4" s="5" t="n"/>
-      <c r="BA4" s="4" t="n"/>
-      <c r="BB4" s="4" t="n"/>
+      <c r="AR4" s="1" t="n"/>
+      <c r="AS4" s="1" t="n"/>
+      <c r="AT4" s="6" t="n"/>
+      <c r="AX4" s="7" t="n"/>
+      <c r="AY4" s="4" t="n"/>
+      <c r="AZ4" s="4" t="n"/>
+      <c r="BA4" s="8" t="n"/>
+      <c r="BB4" s="2" t="n"/>
       <c r="BC4" s="2" t="n"/>
       <c r="BD4" s="2" t="n"/>
-      <c r="BE4" s="7" t="n"/>
-      <c r="BI4" s="8" t="n"/>
-      <c r="BJ4" s="8" t="n"/>
+      <c r="BE4" s="5" t="n"/>
+      <c r="BF4" s="6" t="n"/>
+      <c r="BJ4" s="2" t="n"/>
       <c r="BK4" s="8" t="n"/>
       <c r="BL4" s="8" t="n"/>
-      <c r="BM4" s="3" t="n"/>
-      <c r="BN4" s="4" t="n"/>
+      <c r="BM4" s="6" t="n"/>
+      <c r="BN4" s="5" t="n"/>
       <c r="BO4" s="4" t="n"/>
-      <c r="BP4" s="6" t="n"/>
-      <c r="BQ4" s="6" t="n"/>
+      <c r="BP4" s="1" t="n"/>
+      <c r="BQ4" s="1" t="n"/>
+      <c r="BR4" s="1" t="n"/>
     </row>
     <row r="5">
-      <c r="A5" s="6" t="n"/>
-      <c r="B5" s="6" t="n"/>
+      <c r="A5" s="7" t="n"/>
+      <c r="B5" s="7" t="n"/>
       <c r="C5" s="7" t="n"/>
-      <c r="D5" s="7" t="n"/>
-      <c r="E5" s="7" t="n"/>
-      <c r="F5" s="5" t="n"/>
-      <c r="G5" s="5" t="n"/>
-      <c r="H5" s="5" t="n"/>
-      <c r="I5" s="5" t="n"/>
-      <c r="J5" s="5" t="n"/>
+      <c r="D5" s="6" t="n"/>
+      <c r="E5" s="6" t="n"/>
+      <c r="F5" s="6" t="n"/>
+      <c r="G5" s="6" t="n"/>
+      <c r="H5" s="6" t="n"/>
+      <c r="I5" s="8" t="n"/>
+      <c r="J5" s="8" t="n"/>
       <c r="M5" s="7" t="n"/>
       <c r="N5" s="7" t="n"/>
       <c r="O5" s="7" t="n"/>
-      <c r="P5" s="8" t="n"/>
-      <c r="Q5" s="8" t="n"/>
+      <c r="P5" s="4" t="n"/>
+      <c r="Q5" s="5" t="n"/>
       <c r="R5" s="8" t="n"/>
       <c r="S5" s="8" t="n"/>
-      <c r="T5" s="6" t="n"/>
-      <c r="U5" s="6" t="n"/>
+      <c r="T5" s="2" t="n"/>
+      <c r="U5" s="2" t="n"/>
       <c r="V5" s="6" t="n"/>
-      <c r="Y5" s="3" t="n"/>
-      <c r="Z5" s="1" t="n"/>
-      <c r="AA5" s="1" t="n"/>
-      <c r="AB5" s="1" t="n"/>
-      <c r="AC5" s="2" t="n"/>
-      <c r="AD5" s="2" t="n"/>
-      <c r="AE5" s="2" t="n"/>
-      <c r="AF5" s="7" t="n"/>
-      <c r="AG5" s="7" t="n"/>
-      <c r="AH5" s="7" t="n"/>
-      <c r="AK5" s="3" t="n"/>
-      <c r="AL5" s="3" t="n"/>
-      <c r="AM5" s="3" t="n"/>
-      <c r="AN5" s="3" t="n"/>
-      <c r="AO5" s="3" t="n"/>
-      <c r="AP5" s="4" t="n"/>
-      <c r="AQ5" s="4" t="n"/>
-      <c r="AR5" s="6" t="n"/>
-      <c r="AS5" s="6" t="n"/>
+      <c r="Y5" s="7" t="n"/>
+      <c r="Z5" s="7" t="n"/>
+      <c r="AA5" s="2" t="n"/>
+      <c r="AB5" s="6" t="n"/>
+      <c r="AC5" s="6" t="n"/>
+      <c r="AD5" s="6" t="n"/>
+      <c r="AE5" s="6" t="n"/>
+      <c r="AF5" s="6" t="n"/>
+      <c r="AG5" s="8" t="n"/>
+      <c r="AH5" s="8" t="n"/>
+      <c r="AK5" s="2" t="n"/>
+      <c r="AL5" s="2" t="n"/>
+      <c r="AM5" s="8" t="n"/>
+      <c r="AN5" s="8" t="n"/>
+      <c r="AO5" s="5" t="n"/>
+      <c r="AP5" s="5" t="n"/>
+      <c r="AQ5" s="1" t="n"/>
+      <c r="AR5" s="1" t="n"/>
+      <c r="AS5" s="1" t="n"/>
       <c r="AT5" s="6" t="n"/>
-      <c r="AW5" s="3" t="n"/>
-      <c r="AX5" s="1" t="n"/>
-      <c r="AY5" s="5" t="n"/>
-      <c r="AZ5" s="5" t="n"/>
+      <c r="AW5" s="7" t="n"/>
+      <c r="AX5" s="7" t="n"/>
+      <c r="AY5" s="7" t="n"/>
+      <c r="AZ5" s="4" t="n"/>
       <c r="BA5" s="5" t="n"/>
       <c r="BB5" s="5" t="n"/>
       <c r="BC5" s="5" t="n"/>
-      <c r="BD5" s="7" t="n"/>
-      <c r="BE5" s="7" t="n"/>
-      <c r="BF5" s="7" t="n"/>
-      <c r="BI5" s="3" t="n"/>
-      <c r="BJ5" s="3" t="n"/>
-      <c r="BK5" s="3" t="n"/>
-      <c r="BL5" s="3" t="n"/>
-      <c r="BM5" s="3" t="n"/>
-      <c r="BN5" s="4" t="n"/>
-      <c r="BO5" s="4" t="n"/>
-      <c r="BP5" s="6" t="n"/>
-      <c r="BQ5" s="6" t="n"/>
-      <c r="BR5" s="6" t="n"/>
+      <c r="BD5" s="5" t="n"/>
+      <c r="BE5" s="5" t="n"/>
+      <c r="BF5" s="6" t="n"/>
+      <c r="BI5" s="2" t="n"/>
+      <c r="BJ5" s="2" t="n"/>
+      <c r="BK5" s="8" t="n"/>
+      <c r="BL5" s="8" t="n"/>
+      <c r="BM5" s="6" t="n"/>
+      <c r="BN5" s="5" t="n"/>
+      <c r="BO5" s="5" t="n"/>
+      <c r="BP5" s="5" t="n"/>
+      <c r="BQ5" s="5" t="n"/>
+      <c r="BR5" s="5" t="n"/>
     </row>
     <row r="6"/>
     <row r="7"/>
     <row r="8">
-      <c r="A8" s="5" t="n"/>
-      <c r="B8" s="8" t="n"/>
-      <c r="C8" s="8" t="n"/>
+      <c r="A8" s="3" t="n"/>
+      <c r="B8" s="3" t="n"/>
+      <c r="C8" s="3" t="n"/>
       <c r="E8" s="6" t="n"/>
-      <c r="F8" s="6" t="n"/>
+      <c r="F8" s="4" t="n"/>
       <c r="G8" s="4" t="n"/>
-      <c r="H8" s="4" t="n"/>
-      <c r="I8" s="4" t="n"/>
-      <c r="J8" s="4" t="n"/>
-      <c r="M8" s="1" t="n"/>
-      <c r="N8" s="1" t="n"/>
-      <c r="O8" s="1" t="n"/>
-      <c r="Q8" s="4" t="n"/>
-      <c r="R8" s="4" t="n"/>
-      <c r="S8" s="8" t="n"/>
-      <c r="T8" s="8" t="n"/>
-      <c r="U8" s="8" t="n"/>
-      <c r="V8" s="8" t="n"/>
-      <c r="Y8" s="4" t="n"/>
-      <c r="Z8" s="4" t="n"/>
-      <c r="AA8" s="3" t="n"/>
-      <c r="AC8" s="5" t="n"/>
-      <c r="AD8" s="5" t="n"/>
-      <c r="AE8" s="5" t="n"/>
-      <c r="AF8" s="5" t="n"/>
-      <c r="AG8" s="5" t="n"/>
-      <c r="AH8" s="6" t="n"/>
+      <c r="H8" s="7" t="n"/>
+      <c r="J8" s="7" t="n"/>
+      <c r="M8" s="3" t="n"/>
+      <c r="N8" s="3" t="n"/>
+      <c r="O8" s="3" t="n"/>
+      <c r="Q8" s="5" t="n"/>
+      <c r="R8" s="5" t="n"/>
+      <c r="S8" s="7" t="n"/>
+      <c r="T8" s="7" t="n"/>
+      <c r="V8" s="6" t="n"/>
     </row>
     <row r="9">
-      <c r="A9" s="5" t="n"/>
-      <c r="B9" s="5" t="n"/>
-      <c r="C9" s="8" t="n"/>
-      <c r="D9" s="1" t="n"/>
+      <c r="A9" s="2" t="n"/>
+      <c r="B9" s="3" t="n"/>
+      <c r="C9" s="3" t="n"/>
+      <c r="D9" s="8" t="n"/>
       <c r="E9" s="6" t="n"/>
       <c r="F9" s="6" t="n"/>
-      <c r="G9" s="2" t="n"/>
-      <c r="H9" s="2" t="n"/>
-      <c r="I9" s="4" t="n"/>
-      <c r="J9" s="4" t="n"/>
-      <c r="M9" s="1" t="n"/>
-      <c r="N9" s="1" t="n"/>
-      <c r="O9" s="4" t="n"/>
-      <c r="P9" s="4" t="n"/>
-      <c r="Q9" s="4" t="n"/>
+      <c r="G9" s="4" t="n"/>
+      <c r="H9" s="7" t="n"/>
+      <c r="I9" s="7" t="n"/>
+      <c r="J9" s="7" t="n"/>
+      <c r="M9" s="2" t="n"/>
+      <c r="N9" s="3" t="n"/>
+      <c r="O9" s="3" t="n"/>
+      <c r="P9" s="8" t="n"/>
+      <c r="Q9" s="5" t="n"/>
       <c r="R9" s="4" t="n"/>
-      <c r="S9" s="8" t="n"/>
+      <c r="S9" s="4" t="n"/>
       <c r="T9" s="7" t="n"/>
-      <c r="U9" s="8" t="n"/>
-      <c r="V9" s="7" t="n"/>
-      <c r="Y9" s="4" t="n"/>
-      <c r="Z9" s="4" t="n"/>
-      <c r="AA9" s="3" t="n"/>
-      <c r="AB9" s="3" t="n"/>
-      <c r="AC9" s="3" t="n"/>
-      <c r="AD9" s="3" t="n"/>
-      <c r="AE9" s="3" t="n"/>
-      <c r="AF9" s="5" t="n"/>
-      <c r="AG9" s="6" t="n"/>
-      <c r="AH9" s="6" t="n"/>
+      <c r="U9" s="6" t="n"/>
+      <c r="V9" s="6" t="n"/>
     </row>
     <row r="10">
-      <c r="A10" s="5" t="n"/>
-      <c r="B10" s="8" t="n"/>
-      <c r="C10" s="8" t="n"/>
-      <c r="D10" s="1" t="n"/>
-      <c r="E10" s="1" t="n"/>
-      <c r="F10" s="6" t="n"/>
-      <c r="H10" s="2" t="n"/>
-      <c r="I10" s="7" t="n"/>
-      <c r="J10" s="7" t="n"/>
-      <c r="M10" s="1" t="n"/>
-      <c r="N10" s="6" t="n"/>
-      <c r="O10" s="6" t="n"/>
-      <c r="P10" s="2" t="n"/>
-      <c r="Q10" s="2" t="n"/>
-      <c r="R10" s="2" t="n"/>
+      <c r="A10" s="2" t="n"/>
+      <c r="B10" s="2" t="n"/>
+      <c r="C10" s="3" t="n"/>
+      <c r="D10" s="8" t="n"/>
+      <c r="E10" s="6" t="n"/>
+      <c r="F10" s="4" t="n"/>
+      <c r="G10" s="4" t="n"/>
+      <c r="H10" s="7" t="n"/>
+      <c r="I10" s="1" t="n"/>
+      <c r="J10" s="1" t="n"/>
+      <c r="M10" s="2" t="n"/>
+      <c r="N10" s="2" t="n"/>
+      <c r="O10" s="3" t="n"/>
+      <c r="P10" s="8" t="n"/>
+      <c r="Q10" s="5" t="n"/>
+      <c r="R10" s="4" t="n"/>
+      <c r="S10" s="7" t="n"/>
       <c r="T10" s="7" t="n"/>
       <c r="U10" s="7" t="n"/>
-      <c r="V10" s="7" t="n"/>
-      <c r="Y10" s="4" t="n"/>
-      <c r="Z10" s="7" t="n"/>
-      <c r="AA10" s="7" t="n"/>
-      <c r="AB10" s="2" t="n"/>
-      <c r="AC10" s="2" t="n"/>
-      <c r="AD10" s="2" t="n"/>
-      <c r="AF10" s="1" t="n"/>
-      <c r="AG10" s="6" t="n"/>
-      <c r="AH10" s="6" t="n"/>
+      <c r="V10" s="6" t="n"/>
     </row>
     <row r="11">
-      <c r="A11" s="5" t="n"/>
-      <c r="B11" s="3" t="n"/>
+      <c r="B11" s="2" t="n"/>
       <c r="C11" s="8" t="n"/>
-      <c r="D11" s="1" t="n"/>
-      <c r="E11" s="1" t="n"/>
-      <c r="F11" s="1" t="n"/>
-      <c r="G11" s="2" t="n"/>
-      <c r="H11" s="2" t="n"/>
-      <c r="I11" s="7" t="n"/>
-      <c r="M11" s="6" t="n"/>
-      <c r="N11" s="6" t="n"/>
-      <c r="O11" s="6" t="n"/>
-      <c r="P11" s="2" t="n"/>
-      <c r="Q11" s="3" t="n"/>
-      <c r="R11" s="2" t="n"/>
-      <c r="S11" s="2" t="n"/>
-      <c r="T11" s="7" t="n"/>
-      <c r="U11" s="5" t="n"/>
-      <c r="Y11" s="4" t="n"/>
-      <c r="Z11" s="7" t="n"/>
-      <c r="AA11" s="2" t="n"/>
-      <c r="AB11" s="2" t="n"/>
-      <c r="AC11" s="8" t="n"/>
-      <c r="AD11" s="2" t="n"/>
-      <c r="AE11" s="8" t="n"/>
-      <c r="AF11" s="1" t="n"/>
-      <c r="AG11" s="1" t="n"/>
+      <c r="D11" s="8" t="n"/>
+      <c r="E11" s="6" t="n"/>
+      <c r="F11" s="5" t="n"/>
+      <c r="G11" s="4" t="n"/>
+      <c r="H11" s="1" t="n"/>
+      <c r="I11" s="1" t="n"/>
+      <c r="J11" s="1" t="n"/>
+      <c r="N11" s="2" t="n"/>
+      <c r="O11" s="8" t="n"/>
+      <c r="P11" s="8" t="n"/>
+      <c r="Q11" s="5" t="n"/>
+      <c r="R11" s="4" t="n"/>
+      <c r="S11" s="4" t="n"/>
+      <c r="T11" s="1" t="n"/>
+      <c r="U11" s="1" t="n"/>
+      <c r="V11" s="6" t="n"/>
     </row>
     <row r="12">
-      <c r="A12" s="5" t="n"/>
-      <c r="B12" s="3" t="n"/>
-      <c r="C12" s="3" t="n"/>
-      <c r="D12" s="3" t="n"/>
-      <c r="E12" s="3" t="n"/>
-      <c r="F12" s="3" t="n"/>
-      <c r="G12" s="2" t="n"/>
-      <c r="H12" s="7" t="n"/>
-      <c r="I12" s="7" t="n"/>
-      <c r="J12" s="7" t="n"/>
-      <c r="M12" s="3" t="n"/>
-      <c r="N12" s="3" t="n"/>
-      <c r="O12" s="3" t="n"/>
-      <c r="P12" s="3" t="n"/>
-      <c r="Q12" s="3" t="n"/>
-      <c r="R12" s="5" t="n"/>
-      <c r="S12" s="5" t="n"/>
-      <c r="T12" s="5" t="n"/>
-      <c r="U12" s="5" t="n"/>
-      <c r="V12" s="5" t="n"/>
-      <c r="Y12" s="7" t="n"/>
-      <c r="Z12" s="7" t="n"/>
-      <c r="AA12" s="7" t="n"/>
-      <c r="AB12" s="8" t="n"/>
-      <c r="AC12" s="8" t="n"/>
-      <c r="AD12" s="8" t="n"/>
-      <c r="AE12" s="8" t="n"/>
-      <c r="AF12" s="1" t="n"/>
-      <c r="AG12" s="1" t="n"/>
-      <c r="AH12" s="1" t="n"/>
+      <c r="A12" s="2" t="n"/>
+      <c r="B12" s="2" t="n"/>
+      <c r="C12" s="8" t="n"/>
+      <c r="D12" s="8" t="n"/>
+      <c r="E12" s="6" t="n"/>
+      <c r="F12" s="5" t="n"/>
+      <c r="G12" s="5" t="n"/>
+      <c r="H12" s="5" t="n"/>
+      <c r="I12" s="5" t="n"/>
+      <c r="J12" s="5" t="n"/>
+      <c r="M12" s="2" t="n"/>
+      <c r="N12" s="2" t="n"/>
+      <c r="O12" s="8" t="n"/>
+      <c r="P12" s="8" t="n"/>
+      <c r="Q12" s="5" t="n"/>
+      <c r="R12" s="4" t="n"/>
+      <c r="S12" s="1" t="n"/>
+      <c r="T12" s="1" t="n"/>
+      <c r="U12" s="1" t="n"/>
+      <c r="V12" s="6" t="n"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>